<commit_message>
add: se agregaron las pestañas Chat Bot y Carga de Archivos
</commit_message>
<xml_diff>
--- a/resources/plan_estudios.xlsx
+++ b/resources/plan_estudios.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NUNU\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\G\mesas-examen\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7C2AAFB-839E-4E24-891A-AD30454D550D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EC98231-DFA4-4CF8-B624-350E11589E42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{808B440C-5695-4001-80B4-F6FD3B72B139}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{808B440C-5695-4001-80B4-F6FD3B72B139}"/>
   </bookViews>
   <sheets>
     <sheet name="Carreras" sheetId="1" r:id="rId1"/>
@@ -291,11 +291,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -615,7 +612,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03B471E8-BFFD-4346-BF88-B7DA647A2C51}">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -623,7 +620,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>71</v>
       </c>
     </row>
@@ -659,7 +656,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>71</v>
       </c>
     </row>
@@ -1012,277 +1009,277 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2">
+      <c r="A2" s="1">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+      <c r="A3" s="1">
         <v>6</v>
       </c>
-      <c r="B3" s="2">
-        <v>1</v>
-      </c>
-      <c r="C3" s="2">
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+      <c r="A4" s="1">
         <v>53</v>
       </c>
-      <c r="B4" s="2">
-        <v>1</v>
-      </c>
-      <c r="C4" s="2">
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+      <c r="A5" s="1">
         <v>15</v>
       </c>
-      <c r="B5" s="2">
-        <v>1</v>
-      </c>
-      <c r="C5" s="2">
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+      <c r="A6" s="1">
         <v>11</v>
       </c>
-      <c r="B6" s="2">
-        <v>1</v>
-      </c>
-      <c r="C6" s="2">
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
+      <c r="A7" s="1">
         <v>59</v>
       </c>
-      <c r="B7" s="2">
-        <v>1</v>
-      </c>
-      <c r="C7" s="2">
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
+      <c r="A8" s="1">
         <v>49</v>
       </c>
-      <c r="B8" s="2">
-        <v>1</v>
-      </c>
-      <c r="C8" s="2">
+      <c r="B8" s="1">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
+      <c r="A9" s="1">
         <v>21</v>
       </c>
-      <c r="B9" s="2">
-        <v>1</v>
-      </c>
-      <c r="C9" s="2">
+      <c r="B9" s="1">
+        <v>1</v>
+      </c>
+      <c r="C9" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
+      <c r="A10" s="1">
         <v>36</v>
       </c>
-      <c r="B10" s="2">
-        <v>1</v>
-      </c>
-      <c r="C10" s="2">
+      <c r="B10" s="1">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
+      <c r="A11" s="1">
         <v>14</v>
       </c>
-      <c r="B11" s="2">
-        <v>1</v>
-      </c>
-      <c r="C11" s="2">
+      <c r="B11" s="1">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
+      <c r="A12" s="1">
         <v>24</v>
       </c>
-      <c r="B12" s="2">
-        <v>1</v>
-      </c>
-      <c r="C12" s="2">
+      <c r="B12" s="1">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
+      <c r="A13" s="1">
         <v>54</v>
       </c>
-      <c r="B13" s="2">
-        <v>1</v>
-      </c>
-      <c r="C13" s="2">
+      <c r="B13" s="1">
+        <v>1</v>
+      </c>
+      <c r="C13" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
+      <c r="A14" s="1">
         <v>41</v>
       </c>
-      <c r="B14" s="2">
-        <v>1</v>
-      </c>
-      <c r="C14" s="2">
+      <c r="B14" s="1">
+        <v>1</v>
+      </c>
+      <c r="C14" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
+      <c r="A15" s="1">
         <v>39</v>
       </c>
-      <c r="B15" s="2">
-        <v>1</v>
-      </c>
-      <c r="C15" s="2">
+      <c r="B15" s="1">
+        <v>1</v>
+      </c>
+      <c r="C15" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
+      <c r="A16" s="1">
         <v>42</v>
       </c>
-      <c r="B16" s="2">
-        <v>1</v>
-      </c>
-      <c r="C16" s="2">
+      <c r="B16" s="1">
+        <v>1</v>
+      </c>
+      <c r="C16" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
+      <c r="A17" s="1">
         <v>50</v>
       </c>
-      <c r="B17" s="2">
-        <v>1</v>
-      </c>
-      <c r="C17" s="2">
+      <c r="B17" s="1">
+        <v>1</v>
+      </c>
+      <c r="C17" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
+      <c r="A18" s="1">
         <v>22</v>
       </c>
-      <c r="B18" s="2">
-        <v>1</v>
-      </c>
-      <c r="C18" s="2">
+      <c r="B18" s="1">
+        <v>1</v>
+      </c>
+      <c r="C18" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
+      <c r="A19" s="1">
         <v>32</v>
       </c>
-      <c r="B19" s="2">
-        <v>1</v>
-      </c>
-      <c r="C19" s="2">
+      <c r="B19" s="1">
+        <v>1</v>
+      </c>
+      <c r="C19" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
+      <c r="A20" s="1">
         <v>44</v>
       </c>
-      <c r="B20" s="2">
-        <v>1</v>
-      </c>
-      <c r="C20" s="2">
+      <c r="B20" s="1">
+        <v>1</v>
+      </c>
+      <c r="C20" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
+      <c r="A21" s="1">
         <v>58</v>
       </c>
-      <c r="B21" s="2">
-        <v>1</v>
-      </c>
-      <c r="C21" s="2">
+      <c r="B21" s="1">
+        <v>1</v>
+      </c>
+      <c r="C21" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
+      <c r="A22" s="1">
         <v>13</v>
       </c>
-      <c r="B22" s="2">
-        <v>1</v>
-      </c>
-      <c r="C22" s="2">
+      <c r="B22" s="1">
+        <v>1</v>
+      </c>
+      <c r="C22" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
+      <c r="A23" s="1">
         <v>26</v>
       </c>
-      <c r="B23" s="2">
-        <v>1</v>
-      </c>
-      <c r="C23" s="2">
+      <c r="B23" s="1">
+        <v>1</v>
+      </c>
+      <c r="C23" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="2">
+      <c r="A24" s="1">
         <v>10</v>
       </c>
-      <c r="B24" s="2">
-        <v>1</v>
-      </c>
-      <c r="C24" s="2">
+      <c r="B24" s="1">
+        <v>1</v>
+      </c>
+      <c r="C24" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="2">
+      <c r="A25" s="1">
         <v>52</v>
       </c>
-      <c r="B25" s="2">
-        <v>1</v>
-      </c>
-      <c r="C25" s="2">
+      <c r="B25" s="1">
+        <v>1</v>
+      </c>
+      <c r="C25" s="1">
         <v>3</v>
       </c>
     </row>
@@ -1293,7 +1290,7 @@
       <c r="B26" s="1">
         <v>1</v>
       </c>
-      <c r="C26" s="2">
+      <c r="C26" s="1">
         <v>3</v>
       </c>
     </row>
@@ -1304,7 +1301,7 @@
       <c r="B27" s="1">
         <v>2</v>
       </c>
-      <c r="C27" s="2">
+      <c r="C27" s="1">
         <v>1</v>
       </c>
     </row>
@@ -1315,7 +1312,7 @@
       <c r="B28" s="1">
         <v>2</v>
       </c>
-      <c r="C28" s="2">
+      <c r="C28" s="1">
         <v>1</v>
       </c>
     </row>
@@ -1326,7 +1323,7 @@
       <c r="B29" s="1">
         <v>2</v>
       </c>
-      <c r="C29" s="2">
+      <c r="C29" s="1">
         <v>1</v>
       </c>
     </row>
@@ -1337,7 +1334,7 @@
       <c r="B30" s="1">
         <v>2</v>
       </c>
-      <c r="C30" s="2">
+      <c r="C30" s="1">
         <v>1</v>
       </c>
     </row>
@@ -1348,7 +1345,7 @@
       <c r="B31" s="1">
         <v>2</v>
       </c>
-      <c r="C31" s="2">
+      <c r="C31" s="1">
         <v>1</v>
       </c>
     </row>
@@ -1359,7 +1356,7 @@
       <c r="B32" s="1">
         <v>2</v>
       </c>
-      <c r="C32" s="2">
+      <c r="C32" s="1">
         <v>1</v>
       </c>
     </row>
@@ -1370,7 +1367,7 @@
       <c r="B33" s="1">
         <v>2</v>
       </c>
-      <c r="C33" s="2">
+      <c r="C33" s="1">
         <v>1</v>
       </c>
     </row>
@@ -1381,7 +1378,7 @@
       <c r="B34" s="1">
         <v>2</v>
       </c>
-      <c r="C34" s="2">
+      <c r="C34" s="1">
         <v>2</v>
       </c>
     </row>
@@ -1392,7 +1389,7 @@
       <c r="B35" s="1">
         <v>2</v>
       </c>
-      <c r="C35" s="2">
+      <c r="C35" s="1">
         <v>2</v>
       </c>
     </row>
@@ -1403,7 +1400,7 @@
       <c r="B36" s="1">
         <v>2</v>
       </c>
-      <c r="C36" s="2">
+      <c r="C36" s="1">
         <v>2</v>
       </c>
     </row>
@@ -1414,7 +1411,7 @@
       <c r="B37" s="1">
         <v>2</v>
       </c>
-      <c r="C37" s="2">
+      <c r="C37" s="1">
         <v>2</v>
       </c>
     </row>
@@ -1425,7 +1422,7 @@
       <c r="B38" s="1">
         <v>2</v>
       </c>
-      <c r="C38" s="2">
+      <c r="C38" s="1">
         <v>2</v>
       </c>
     </row>
@@ -1436,7 +1433,7 @@
       <c r="B39" s="1">
         <v>2</v>
       </c>
-      <c r="C39" s="2">
+      <c r="C39" s="1">
         <v>2</v>
       </c>
     </row>
@@ -1447,7 +1444,7 @@
       <c r="B40" s="1">
         <v>2</v>
       </c>
-      <c r="C40" s="2">
+      <c r="C40" s="1">
         <v>2</v>
       </c>
     </row>
@@ -1458,7 +1455,7 @@
       <c r="B41" s="1">
         <v>2</v>
       </c>
-      <c r="C41" s="2">
+      <c r="C41" s="1">
         <v>2</v>
       </c>
     </row>
@@ -1469,7 +1466,7 @@
       <c r="B42" s="1">
         <v>2</v>
       </c>
-      <c r="C42" s="2">
+      <c r="C42" s="1">
         <v>3</v>
       </c>
     </row>
@@ -1480,7 +1477,7 @@
       <c r="B43" s="1">
         <v>2</v>
       </c>
-      <c r="C43" s="2">
+      <c r="C43" s="1">
         <v>3</v>
       </c>
     </row>
@@ -1491,7 +1488,7 @@
       <c r="B44" s="1">
         <v>2</v>
       </c>
-      <c r="C44" s="2">
+      <c r="C44" s="1">
         <v>3</v>
       </c>
     </row>
@@ -1502,7 +1499,7 @@
       <c r="B45" s="1">
         <v>2</v>
       </c>
-      <c r="C45" s="2">
+      <c r="C45" s="1">
         <v>3</v>
       </c>
     </row>
@@ -1513,7 +1510,7 @@
       <c r="B46" s="1">
         <v>2</v>
       </c>
-      <c r="C46" s="2">
+      <c r="C46" s="1">
         <v>3</v>
       </c>
     </row>
@@ -1524,7 +1521,7 @@
       <c r="B47" s="1">
         <v>2</v>
       </c>
-      <c r="C47" s="2">
+      <c r="C47" s="1">
         <v>3</v>
       </c>
     </row>
@@ -1535,7 +1532,7 @@
       <c r="B48" s="1">
         <v>2</v>
       </c>
-      <c r="C48" s="2">
+      <c r="C48" s="1">
         <v>3</v>
       </c>
     </row>
@@ -1546,7 +1543,7 @@
       <c r="B49" s="1">
         <v>2</v>
       </c>
-      <c r="C49" s="2">
+      <c r="C49" s="1">
         <v>3</v>
       </c>
     </row>
@@ -1557,7 +1554,7 @@
       <c r="B50" s="1">
         <v>2</v>
       </c>
-      <c r="C50" s="2">
+      <c r="C50" s="1">
         <v>4</v>
       </c>
     </row>
@@ -1568,7 +1565,7 @@
       <c r="B51" s="1">
         <v>2</v>
       </c>
-      <c r="C51" s="2">
+      <c r="C51" s="1">
         <v>4</v>
       </c>
     </row>
@@ -1579,7 +1576,7 @@
       <c r="B52" s="1">
         <v>2</v>
       </c>
-      <c r="C52" s="2">
+      <c r="C52" s="1">
         <v>4</v>
       </c>
     </row>
@@ -1590,7 +1587,7 @@
       <c r="B53" s="1">
         <v>2</v>
       </c>
-      <c r="C53" s="2">
+      <c r="C53" s="1">
         <v>4</v>
       </c>
     </row>
@@ -1601,7 +1598,7 @@
       <c r="B54" s="1">
         <v>2</v>
       </c>
-      <c r="C54" s="2">
+      <c r="C54" s="1">
         <v>4</v>
       </c>
     </row>
@@ -1612,7 +1609,7 @@
       <c r="B55" s="1">
         <v>2</v>
       </c>
-      <c r="C55" s="2">
+      <c r="C55" s="1">
         <v>4</v>
       </c>
     </row>
@@ -1623,7 +1620,7 @@
       <c r="B56" s="1">
         <v>3</v>
       </c>
-      <c r="C56" s="2">
+      <c r="C56" s="1">
         <v>1</v>
       </c>
     </row>
@@ -1634,7 +1631,7 @@
       <c r="B57" s="1">
         <v>3</v>
       </c>
-      <c r="C57" s="2">
+      <c r="C57" s="1">
         <v>1</v>
       </c>
     </row>
@@ -1645,7 +1642,7 @@
       <c r="B58" s="1">
         <v>3</v>
       </c>
-      <c r="C58" s="2">
+      <c r="C58" s="1">
         <v>1</v>
       </c>
     </row>
@@ -1656,7 +1653,7 @@
       <c r="B59" s="1">
         <v>3</v>
       </c>
-      <c r="C59" s="2">
+      <c r="C59" s="1">
         <v>1</v>
       </c>
     </row>
@@ -1667,7 +1664,7 @@
       <c r="B60" s="1">
         <v>3</v>
       </c>
-      <c r="C60" s="2">
+      <c r="C60" s="1">
         <v>1</v>
       </c>
     </row>
@@ -1678,7 +1675,7 @@
       <c r="B61" s="1">
         <v>3</v>
       </c>
-      <c r="C61" s="2">
+      <c r="C61" s="1">
         <v>1</v>
       </c>
     </row>
@@ -1689,7 +1686,7 @@
       <c r="B62" s="1">
         <v>3</v>
       </c>
-      <c r="C62" s="2">
+      <c r="C62" s="1">
         <v>1</v>
       </c>
     </row>
@@ -1700,7 +1697,7 @@
       <c r="B63" s="1">
         <v>3</v>
       </c>
-      <c r="C63" s="2">
+      <c r="C63" s="1">
         <v>1</v>
       </c>
     </row>
@@ -1711,7 +1708,7 @@
       <c r="B64" s="1">
         <v>3</v>
       </c>
-      <c r="C64" s="2">
+      <c r="C64" s="1">
         <v>2</v>
       </c>
     </row>
@@ -1722,7 +1719,7 @@
       <c r="B65" s="1">
         <v>3</v>
       </c>
-      <c r="C65" s="2">
+      <c r="C65" s="1">
         <v>2</v>
       </c>
     </row>
@@ -1733,7 +1730,7 @@
       <c r="B66" s="1">
         <v>3</v>
       </c>
-      <c r="C66" s="2">
+      <c r="C66" s="1">
         <v>2</v>
       </c>
     </row>
@@ -1744,7 +1741,7 @@
       <c r="B67" s="1">
         <v>3</v>
       </c>
-      <c r="C67" s="2">
+      <c r="C67" s="1">
         <v>2</v>
       </c>
     </row>
@@ -1755,7 +1752,7 @@
       <c r="B68" s="1">
         <v>3</v>
       </c>
-      <c r="C68" s="2">
+      <c r="C68" s="1">
         <v>2</v>
       </c>
     </row>
@@ -1766,7 +1763,7 @@
       <c r="B69" s="1">
         <v>3</v>
       </c>
-      <c r="C69" s="2">
+      <c r="C69" s="1">
         <v>2</v>
       </c>
     </row>
@@ -1777,7 +1774,7 @@
       <c r="B70" s="1">
         <v>3</v>
       </c>
-      <c r="C70" s="2">
+      <c r="C70" s="1">
         <v>2</v>
       </c>
     </row>
@@ -1788,7 +1785,7 @@
       <c r="B71" s="1">
         <v>3</v>
       </c>
-      <c r="C71" s="2">
+      <c r="C71" s="1">
         <v>2</v>
       </c>
     </row>
@@ -1799,7 +1796,7 @@
       <c r="B72" s="1">
         <v>3</v>
       </c>
-      <c r="C72" s="2">
+      <c r="C72" s="1">
         <v>2</v>
       </c>
     </row>
@@ -1810,7 +1807,7 @@
       <c r="B73" s="1">
         <v>3</v>
       </c>
-      <c r="C73" s="2">
+      <c r="C73" s="1">
         <v>3</v>
       </c>
     </row>
@@ -1821,7 +1818,7 @@
       <c r="B74" s="1">
         <v>3</v>
       </c>
-      <c r="C74" s="2">
+      <c r="C74" s="1">
         <v>3</v>
       </c>
     </row>
@@ -1832,7 +1829,7 @@
       <c r="B75" s="1">
         <v>3</v>
       </c>
-      <c r="C75" s="2">
+      <c r="C75" s="1">
         <v>3</v>
       </c>
     </row>
@@ -1843,7 +1840,7 @@
       <c r="B76" s="1">
         <v>3</v>
       </c>
-      <c r="C76" s="2">
+      <c r="C76" s="1">
         <v>3</v>
       </c>
     </row>
@@ -1854,7 +1851,7 @@
       <c r="B77" s="1">
         <v>3</v>
       </c>
-      <c r="C77" s="2">
+      <c r="C77" s="1">
         <v>3</v>
       </c>
     </row>
@@ -1865,7 +1862,7 @@
       <c r="B78" s="1">
         <v>3</v>
       </c>
-      <c r="C78" s="2">
+      <c r="C78" s="1">
         <v>3</v>
       </c>
     </row>
@@ -1876,7 +1873,7 @@
       <c r="B79" s="1">
         <v>3</v>
       </c>
-      <c r="C79" s="2">
+      <c r="C79" s="1">
         <v>3</v>
       </c>
     </row>
@@ -1887,7 +1884,7 @@
       <c r="B80" s="1">
         <v>3</v>
       </c>
-      <c r="C80" s="2">
+      <c r="C80" s="1">
         <v>3</v>
       </c>
     </row>
@@ -1898,7 +1895,7 @@
       <c r="B81" s="1">
         <v>3</v>
       </c>
-      <c r="C81" s="2">
+      <c r="C81" s="1">
         <v>4</v>
       </c>
     </row>
@@ -1909,7 +1906,7 @@
       <c r="B82" s="1">
         <v>3</v>
       </c>
-      <c r="C82" s="2">
+      <c r="C82" s="1">
         <v>4</v>
       </c>
     </row>
@@ -1920,7 +1917,7 @@
       <c r="B83" s="1">
         <v>3</v>
       </c>
-      <c r="C83" s="2">
+      <c r="C83" s="1">
         <v>4</v>
       </c>
     </row>
@@ -1931,7 +1928,7 @@
       <c r="B84" s="1">
         <v>3</v>
       </c>
-      <c r="C84" s="2">
+      <c r="C84" s="1">
         <v>4</v>
       </c>
     </row>
@@ -1942,7 +1939,7 @@
       <c r="B85" s="1">
         <v>3</v>
       </c>
-      <c r="C85" s="2">
+      <c r="C85" s="1">
         <v>4</v>
       </c>
     </row>
@@ -1953,7 +1950,7 @@
       <c r="B86" s="1">
         <v>3</v>
       </c>
-      <c r="C86" s="2">
+      <c r="C86" s="1">
         <v>4</v>
       </c>
     </row>
@@ -1964,9 +1961,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88A76A1B-AB3C-4CFB-8707-E312FB8E7EC1}">
-  <dimension ref="A1:B51"/>
+  <dimension ref="A1:B209"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1975,411 +1974,1675 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+      <c r="A2" s="1">
         <v>10</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+      <c r="A3" s="1">
         <v>10</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+      <c r="A4" s="1">
         <v>10</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+      <c r="A5" s="1">
         <v>11</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+      <c r="A6" s="1">
         <v>11</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
+      <c r="A7" s="1">
         <v>12</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
+      <c r="A8" s="1">
         <v>12</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="1">
         <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
+      <c r="A9" s="1">
         <v>13</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
+      <c r="A10" s="1">
         <v>13</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
+      <c r="A11" s="1">
         <v>13</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="1">
         <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
+      <c r="A12" s="1">
         <v>14</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
+      <c r="A13" s="1">
         <v>14</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
+      <c r="A14" s="1">
         <v>14</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="1">
         <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
+      <c r="A15" s="1">
         <v>15</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
+      <c r="A16" s="1">
         <v>15</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="1">
         <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
+      <c r="A17" s="1">
         <v>15</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
+      <c r="A18" s="1">
         <v>16</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
+      <c r="A19" s="1">
         <v>16</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
+      <c r="A20" s="1">
         <v>16</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
+      <c r="A21" s="1">
         <v>16</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
+      <c r="A22" s="1">
         <v>16</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B22" s="1">
         <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
+      <c r="A23" s="1">
         <v>16</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B23" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="2">
+      <c r="A24" s="1">
         <v>16</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B24" s="1">
         <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="2">
+      <c r="A25" s="1">
         <v>16</v>
       </c>
-      <c r="B25" s="2">
+      <c r="B25" s="1">
         <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="2">
+      <c r="A26" s="1">
         <v>18</v>
       </c>
-      <c r="B26" s="2">
+      <c r="B26" s="1">
         <v>15</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="2">
+      <c r="A27" s="1">
         <v>19</v>
       </c>
-      <c r="B27" s="2">
+      <c r="B27" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="2">
+      <c r="A28" s="1">
         <v>20</v>
       </c>
-      <c r="B28" s="2">
+      <c r="B28" s="1">
         <v>11</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="2">
+      <c r="A29" s="1">
         <v>20</v>
       </c>
-      <c r="B29" s="2">
+      <c r="B29" s="1">
         <v>13</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="2">
+      <c r="A30" s="1">
         <v>20</v>
       </c>
-      <c r="B30" s="2">
+      <c r="B30" s="1">
         <v>14</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="2">
+      <c r="A31" s="1">
         <v>21</v>
       </c>
-      <c r="B31" s="2">
+      <c r="B31" s="1">
         <v>9</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="2">
+      <c r="A32" s="1">
         <v>21</v>
       </c>
-      <c r="B32" s="2">
+      <c r="B32" s="1">
         <v>14</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="2">
+      <c r="A33" s="1">
         <v>21</v>
       </c>
-      <c r="B33" s="2">
+      <c r="B33" s="1">
         <v>15</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="2">
+      <c r="A34" s="1">
         <v>22</v>
       </c>
-      <c r="B34" s="2">
+      <c r="B34" s="1">
         <v>14</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="2">
+      <c r="A35" s="1">
         <v>22</v>
       </c>
-      <c r="B35" s="2">
+      <c r="B35" s="1">
         <v>15</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="2">
+      <c r="A36" s="1">
         <v>23</v>
       </c>
-      <c r="B36" s="2">
+      <c r="B36" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="2">
+      <c r="A37" s="1">
         <v>23</v>
       </c>
-      <c r="B37" s="2">
+      <c r="B37" s="1">
         <v>12</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="2">
+      <c r="A38" s="1">
         <v>23</v>
       </c>
-      <c r="B38" s="2">
+      <c r="B38" s="1">
         <v>13</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="2">
+      <c r="A39" s="1">
         <v>24</v>
       </c>
-      <c r="B39" s="2">
+      <c r="B39" s="1">
         <v>11</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="2">
+      <c r="A40" s="1">
         <v>24</v>
       </c>
-      <c r="B40" s="2">
+      <c r="B40" s="1">
         <v>13</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="2">
+      <c r="A41" s="1">
         <v>24</v>
       </c>
-      <c r="B41" s="2">
+      <c r="B41" s="1">
         <v>14</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="2">
+      <c r="A42" s="1">
         <v>24</v>
       </c>
-      <c r="B42" s="2">
+      <c r="B42" s="1">
         <v>15</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="2">
+      <c r="A43" s="1">
         <v>25</v>
       </c>
-      <c r="B43" s="2">
+      <c r="B43" s="1">
         <v>9</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="2">
+      <c r="A44" s="1">
         <v>25</v>
       </c>
-      <c r="B44" s="2">
+      <c r="B44" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="2">
+      <c r="A45" s="1">
         <v>25</v>
       </c>
-      <c r="B45" s="2">
+      <c r="B45" s="1">
         <v>11</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="2">
+      <c r="A46" s="1">
         <v>25</v>
       </c>
-      <c r="B46" s="2">
+      <c r="B46" s="1">
         <v>12</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="2">
+      <c r="A47" s="1">
         <v>25</v>
       </c>
-      <c r="B47" s="2">
+      <c r="B47" s="1">
         <v>13</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="2">
+      <c r="A48" s="1">
         <v>25</v>
       </c>
-      <c r="B48" s="2">
+      <c r="B48" s="1">
         <v>14</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="2">
+      <c r="A49" s="1">
         <v>25</v>
       </c>
-      <c r="B49" s="2">
+      <c r="B49" s="1">
         <v>15</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="2">
+      <c r="A50" s="1">
         <v>25</v>
       </c>
-      <c r="B50" s="2">
+      <c r="B50" s="1">
         <v>16</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="2">
+      <c r="A51" s="1">
         <v>25</v>
       </c>
-      <c r="B51" s="2">
+      <c r="B51" s="1">
         <v>17</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
+        <v>33</v>
+      </c>
+      <c r="B52" s="1">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
+        <v>36</v>
+      </c>
+      <c r="B53" s="1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
+        <v>37</v>
+      </c>
+      <c r="B54" s="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
+        <v>38</v>
+      </c>
+      <c r="B55" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
+        <v>39</v>
+      </c>
+      <c r="B56" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
+        <v>40</v>
+      </c>
+      <c r="B57" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="1">
+        <v>43</v>
+      </c>
+      <c r="B58" s="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="1">
+        <v>44</v>
+      </c>
+      <c r="B59" s="1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="1">
+        <v>44</v>
+      </c>
+      <c r="B60" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="1">
+        <v>44</v>
+      </c>
+      <c r="B61" s="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="1">
+        <v>44</v>
+      </c>
+      <c r="B62" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="1">
+        <v>44</v>
+      </c>
+      <c r="B63" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="1">
+        <v>44</v>
+      </c>
+      <c r="B64" s="1">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="1">
+        <v>44</v>
+      </c>
+      <c r="B65" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="1">
+        <v>44</v>
+      </c>
+      <c r="B66" s="1">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="1">
+        <v>45</v>
+      </c>
+      <c r="B67" s="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="1">
+        <v>45</v>
+      </c>
+      <c r="B68" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="1">
+        <v>45</v>
+      </c>
+      <c r="B69" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="1">
+        <v>45</v>
+      </c>
+      <c r="B70" s="1">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" s="1">
+        <v>45</v>
+      </c>
+      <c r="B71" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" s="1">
+        <v>45</v>
+      </c>
+      <c r="B72" s="1">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" s="1">
+        <v>46</v>
+      </c>
+      <c r="B73" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" s="1">
+        <v>46</v>
+      </c>
+      <c r="B74" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" s="1">
+        <v>47</v>
+      </c>
+      <c r="B75" s="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" s="1">
+        <v>47</v>
+      </c>
+      <c r="B76" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" s="1">
+        <v>47</v>
+      </c>
+      <c r="B77" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" s="1">
+        <v>48</v>
+      </c>
+      <c r="B78" s="1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" s="1">
+        <v>48</v>
+      </c>
+      <c r="B79" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" s="1">
+        <v>48</v>
+      </c>
+      <c r="B80" s="1">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" s="1">
+        <v>48</v>
+      </c>
+      <c r="B81" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" s="1">
+        <v>48</v>
+      </c>
+      <c r="B82" s="1">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" s="1">
+        <v>48</v>
+      </c>
+      <c r="B83" s="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" s="1">
+        <v>49</v>
+      </c>
+      <c r="B84" s="1">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" s="1">
+        <v>50</v>
+      </c>
+      <c r="B85" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" s="1">
+        <v>50</v>
+      </c>
+      <c r="B86" s="1">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" s="1">
+        <v>51</v>
+      </c>
+      <c r="B87" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" s="1">
+        <v>51</v>
+      </c>
+      <c r="B88" s="1">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" s="1">
+        <v>52</v>
+      </c>
+      <c r="B89" s="1">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" s="1">
+        <v>52</v>
+      </c>
+      <c r="B90" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" s="1">
+        <v>52</v>
+      </c>
+      <c r="B91" s="1">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" s="1">
+        <v>52</v>
+      </c>
+      <c r="B92" s="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" s="1">
+        <v>52</v>
+      </c>
+      <c r="B93" s="1">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" s="1">
+        <v>52</v>
+      </c>
+      <c r="B94" s="1">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" s="1">
+        <v>53</v>
+      </c>
+      <c r="B95" s="1">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" s="1">
+        <v>53</v>
+      </c>
+      <c r="B96" s="1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" s="1">
+        <v>53</v>
+      </c>
+      <c r="B97" s="1">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" s="1">
+        <v>53</v>
+      </c>
+      <c r="B98" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" s="1">
+        <v>53</v>
+      </c>
+      <c r="B99" s="1">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" s="1">
+        <v>53</v>
+      </c>
+      <c r="B100" s="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" s="1">
+        <v>53</v>
+      </c>
+      <c r="B101" s="1">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" s="1">
+        <v>53</v>
+      </c>
+      <c r="B102" s="1">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" s="1">
+        <v>53</v>
+      </c>
+      <c r="B103" s="1">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" s="1">
+        <v>53</v>
+      </c>
+      <c r="B104" s="1">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" s="1">
+        <v>53</v>
+      </c>
+      <c r="B105" s="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" s="1">
+        <v>53</v>
+      </c>
+      <c r="B106" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" s="1">
+        <v>53</v>
+      </c>
+      <c r="B107" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" s="1">
+        <v>53</v>
+      </c>
+      <c r="B108" s="1">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" s="1">
+        <v>53</v>
+      </c>
+      <c r="B109" s="1">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" s="1">
+        <v>54</v>
+      </c>
+      <c r="B110" s="1">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" s="1">
+        <v>54</v>
+      </c>
+      <c r="B111" s="1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" s="1">
+        <v>54</v>
+      </c>
+      <c r="B112" s="1">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" s="1">
+        <v>54</v>
+      </c>
+      <c r="B113" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114" s="1">
+        <v>54</v>
+      </c>
+      <c r="B114" s="1">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115" s="1">
+        <v>54</v>
+      </c>
+      <c r="B115" s="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116" s="1">
+        <v>54</v>
+      </c>
+      <c r="B116" s="1">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117" s="1">
+        <v>54</v>
+      </c>
+      <c r="B117" s="1">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118" s="1">
+        <v>54</v>
+      </c>
+      <c r="B118" s="1">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119" s="1">
+        <v>54</v>
+      </c>
+      <c r="B119" s="1">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120" s="1">
+        <v>54</v>
+      </c>
+      <c r="B120" s="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121" s="1">
+        <v>54</v>
+      </c>
+      <c r="B121" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122" s="1">
+        <v>54</v>
+      </c>
+      <c r="B122" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123" s="1">
+        <v>54</v>
+      </c>
+      <c r="B123" s="1">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124" s="1">
+        <v>54</v>
+      </c>
+      <c r="B124" s="1">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125" s="1">
+        <v>54</v>
+      </c>
+      <c r="B125" s="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A126" s="1">
+        <v>54</v>
+      </c>
+      <c r="B126" s="1">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A127" s="1">
+        <v>54</v>
+      </c>
+      <c r="B127" s="1">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128" s="1">
+        <v>54</v>
+      </c>
+      <c r="B128" s="1">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129" s="1">
+        <v>66</v>
+      </c>
+      <c r="B129" s="1">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130" s="1">
+        <v>67</v>
+      </c>
+      <c r="B130" s="1">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131" s="1">
+        <v>69</v>
+      </c>
+      <c r="B131" s="1">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132" s="1">
+        <v>70</v>
+      </c>
+      <c r="B132" s="1">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133" s="1">
+        <v>70</v>
+      </c>
+      <c r="B133" s="1">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134" s="1">
+        <v>71</v>
+      </c>
+      <c r="B134" s="1">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135" s="1">
+        <v>72</v>
+      </c>
+      <c r="B135" s="1">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136" s="1">
+        <v>73</v>
+      </c>
+      <c r="B136" s="1">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137" s="1">
+        <v>73</v>
+      </c>
+      <c r="B137" s="1">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A138" s="1">
+        <v>74</v>
+      </c>
+      <c r="B138" s="1">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A139" s="1">
+        <v>74</v>
+      </c>
+      <c r="B139" s="1">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A140" s="1">
+        <v>74</v>
+      </c>
+      <c r="B140" s="1">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A141" s="1">
+        <v>75</v>
+      </c>
+      <c r="B141" s="1">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A142" s="1">
+        <v>75</v>
+      </c>
+      <c r="B142" s="1">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A143" s="1">
+        <v>75</v>
+      </c>
+      <c r="B143" s="1">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A144" s="1">
+        <v>75</v>
+      </c>
+      <c r="B144" s="1">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A145" s="1">
+        <v>75</v>
+      </c>
+      <c r="B145" s="1">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A146" s="1">
+        <v>75</v>
+      </c>
+      <c r="B146" s="1">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A147" s="1">
+        <v>75</v>
+      </c>
+      <c r="B147" s="1">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A148" s="1">
+        <v>76</v>
+      </c>
+      <c r="B148" s="1">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A149" s="1">
+        <v>76</v>
+      </c>
+      <c r="B149" s="1">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A150" s="1">
+        <v>76</v>
+      </c>
+      <c r="B150" s="1">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A151" s="1">
+        <v>76</v>
+      </c>
+      <c r="B151" s="1">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A152" s="1">
+        <v>77</v>
+      </c>
+      <c r="B152" s="1">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A153" s="1">
+        <v>77</v>
+      </c>
+      <c r="B153" s="1">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A154" s="1">
+        <v>79</v>
+      </c>
+      <c r="B154" s="1">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A155" s="1">
+        <v>79</v>
+      </c>
+      <c r="B155" s="1">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A156" s="1">
+        <v>79</v>
+      </c>
+      <c r="B156" s="1">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A157" s="1">
+        <v>79</v>
+      </c>
+      <c r="B157" s="1">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A158" s="1">
+        <v>79</v>
+      </c>
+      <c r="B158" s="1">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A159" s="1">
+        <v>79</v>
+      </c>
+      <c r="B159" s="1">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A160" s="1">
+        <v>79</v>
+      </c>
+      <c r="B160" s="1">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A161" s="1">
+        <v>79</v>
+      </c>
+      <c r="B161" s="1">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A162" s="1">
+        <v>79</v>
+      </c>
+      <c r="B162" s="1">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A163" s="1">
+        <v>79</v>
+      </c>
+      <c r="B163" s="1">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A164" s="1">
+        <v>80</v>
+      </c>
+      <c r="B164" s="1">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A165" s="1">
+        <v>80</v>
+      </c>
+      <c r="B165" s="1">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A166" s="1">
+        <v>81</v>
+      </c>
+      <c r="B166" s="1">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A167" s="1">
+        <v>81</v>
+      </c>
+      <c r="B167" s="1">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A168" s="1">
+        <v>81</v>
+      </c>
+      <c r="B168" s="1">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A169" s="1">
+        <v>81</v>
+      </c>
+      <c r="B169" s="1">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A170" s="1">
+        <v>82</v>
+      </c>
+      <c r="B170" s="1">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A171" s="1">
+        <v>82</v>
+      </c>
+      <c r="B171" s="1">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A172" s="1">
+        <v>83</v>
+      </c>
+      <c r="B172" s="1">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A173" s="1">
+        <v>84</v>
+      </c>
+      <c r="B173" s="1">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A174" s="1">
+        <v>84</v>
+      </c>
+      <c r="B174" s="1">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A175" s="1">
+        <v>84</v>
+      </c>
+      <c r="B175" s="1">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A176" s="1">
+        <v>84</v>
+      </c>
+      <c r="B176" s="1">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A177" s="1">
+        <v>84</v>
+      </c>
+      <c r="B177" s="1">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A178" s="1">
+        <v>84</v>
+      </c>
+      <c r="B178" s="1">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A179" s="1">
+        <v>84</v>
+      </c>
+      <c r="B179" s="1">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A180" s="1">
+        <v>84</v>
+      </c>
+      <c r="B180" s="1">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A181" s="1">
+        <v>84</v>
+      </c>
+      <c r="B181" s="1">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A182" s="1">
+        <v>84</v>
+      </c>
+      <c r="B182" s="1">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A183" s="1">
+        <v>84</v>
+      </c>
+      <c r="B183" s="1">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A184" s="1">
+        <v>84</v>
+      </c>
+      <c r="B184" s="1">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A185" s="1">
+        <v>84</v>
+      </c>
+      <c r="B185" s="1">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A186" s="1">
+        <v>84</v>
+      </c>
+      <c r="B186" s="1">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A187" s="1">
+        <v>84</v>
+      </c>
+      <c r="B187" s="1">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A188" s="1">
+        <v>84</v>
+      </c>
+      <c r="B188" s="1">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A189" s="1">
+        <v>84</v>
+      </c>
+      <c r="B189" s="1">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A190" s="1">
+        <v>85</v>
+      </c>
+      <c r="B190" s="1">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A191" s="1">
+        <v>85</v>
+      </c>
+      <c r="B191" s="1">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A192" s="1">
+        <v>85</v>
+      </c>
+      <c r="B192" s="1">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A193" s="1">
+        <v>85</v>
+      </c>
+      <c r="B193" s="1">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A194" s="1">
+        <v>85</v>
+      </c>
+      <c r="B194" s="1">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A195" s="1">
+        <v>85</v>
+      </c>
+      <c r="B195" s="1">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A196" s="1">
+        <v>85</v>
+      </c>
+      <c r="B196" s="1">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A197" s="1">
+        <v>85</v>
+      </c>
+      <c r="B197" s="1">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A198" s="1">
+        <v>85</v>
+      </c>
+      <c r="B198" s="1">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A199" s="1">
+        <v>85</v>
+      </c>
+      <c r="B199" s="1">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A200" s="1">
+        <v>85</v>
+      </c>
+      <c r="B200" s="1">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A201" s="1">
+        <v>85</v>
+      </c>
+      <c r="B201" s="1">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A202" s="1">
+        <v>85</v>
+      </c>
+      <c r="B202" s="1">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A203" s="1">
+        <v>85</v>
+      </c>
+      <c r="B203" s="1">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A204" s="1">
+        <v>85</v>
+      </c>
+      <c r="B204" s="1">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A205" s="1">
+        <v>85</v>
+      </c>
+      <c r="B205" s="1">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A206" s="1">
+        <v>85</v>
+      </c>
+      <c r="B206" s="1">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A207" s="1">
+        <v>85</v>
+      </c>
+      <c r="B207" s="1">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A208" s="1">
+        <v>85</v>
+      </c>
+      <c r="B208" s="1">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A209" s="1">
+        <v>85</v>
+      </c>
+      <c r="B209" s="1">
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
restructuring: restructuración del código e implementación del chatbot
</commit_message>
<xml_diff>
--- a/resources/plan_estudios.xlsx
+++ b/resources/plan_estudios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\G\mesas-examen\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EC98231-DFA4-4CF8-B624-350E11589E42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{044B2CBF-D816-4242-B60D-ED39E69B1526}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{808B440C-5695-4001-80B4-F6FD3B72B139}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{808B440C-5695-4001-80B4-F6FD3B72B139}"/>
   </bookViews>
   <sheets>
     <sheet name="Carreras" sheetId="1" r:id="rId1"/>
@@ -279,7 +279,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -287,13 +287,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -612,15 +630,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03B471E8-BFFD-4346-BF88-B7DA647A2C51}">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="48.140625" customWidth="1"/>
+    <col min="1" max="1" width="48.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>71</v>
       </c>
     </row>
@@ -652,11 +670,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="49.85546875" customWidth="1"/>
+    <col min="1" max="1" width="50.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>71</v>
       </c>
     </row>
@@ -1009,13 +1027,13 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>73</v>
       </c>
     </row>
@@ -1963,21 +1981,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88A76A1B-AB3C-4CFB-8707-E312FB8E7EC1}">
   <dimension ref="A1:B209"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>75</v>
       </c>
     </row>

</xml_diff>